<commit_message>
Preliminary data visualization, PCA.
</commit_message>
<xml_diff>
--- a/data/tentative_final.xlsx
+++ b/data/tentative_final.xlsx
@@ -476,7 +476,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>poverty_rate_%</t>
+          <t>poverty_rate</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -496,7 +496,7 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Vacant_Rate</t>
+          <t>vacancy_rate</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -521,7 +521,7 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Median_Age_(years)</t>
+          <t>median_age</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">

</xml_diff>